<commit_message>
updating RStudio with proper git location
</commit_message>
<xml_diff>
--- a/Coded_WF_10_13_2015v2.xlsx
+++ b/Coded_WF_10_13_2015v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27620" yWindow="5600" windowWidth="21380" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="28360" yWindow="2900" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3451,8 +3451,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3648,7 +3652,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="179">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3736,6 +3740,8 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3823,6 +3829,8 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4154,10 +4162,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CN401"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="720"/>
-      <selection sqref="A1:XFD1048576"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection activeCell="BF1" sqref="BF1:BF1048576"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -83666,7 +83674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>

</xml_diff>